<commit_message>
Correcting support_fraction for EE and creating exponential_list for max_samples
</commit_message>
<xml_diff>
--- a/results/OneClassSVM.xlsx
+++ b/results/OneClassSVM.xlsx
@@ -448,7 +448,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>37.98030033111572</v>
+        <v>37.98214650154114</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.03460788726806641</v>
+        <v>0.03340821266174317</v>
       </c>
     </row>
     <row r="4">

</xml_diff>